<commit_message>
June 10, 2024, 10:30 PM
</commit_message>
<xml_diff>
--- a/NOTE.xlsx
+++ b/NOTE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255"/>
+    <workbookView windowWidth="28800" windowHeight="11500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,16 +31,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -48,7 +48,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -56,14 +56,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -71,7 +71,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -79,7 +79,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -87,7 +87,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -95,7 +95,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -103,14 +103,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -118,7 +118,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -126,7 +126,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -134,14 +134,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -149,42 +149,42 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -494,19 +494,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -645,55 +645,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -734,8 +734,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="447675" y="1362075"/>
-          <a:ext cx="5762625" cy="1676400"/>
+          <a:off x="447675" y="1655445"/>
+          <a:ext cx="6174105" cy="2095500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -776,8 +776,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="628650" y="3219450"/>
-          <a:ext cx="5095875" cy="1000125"/>
+          <a:off x="628650" y="3973830"/>
+          <a:ext cx="5461635" cy="1251585"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -818,8 +818,50 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="685800" y="4800600"/>
-          <a:ext cx="3162300" cy="1609725"/>
+          <a:off x="731520" y="5974080"/>
+          <a:ext cx="3345180" cy="1986915"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>635</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>400685</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>69215</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="635" y="10390505"/>
+          <a:ext cx="11372850" cy="5680710"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -836,32 +878,158 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>43180</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="图片 5"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
+        <a:blip r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="7372350"/>
-          <a:ext cx="10687050" cy="4591050"/>
+          <a:off x="0" y="15575280"/>
+          <a:ext cx="7607300" cy="5803900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>420370</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>113665</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>331470</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>116205</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="420370" y="8434705"/>
+          <a:ext cx="14541500" cy="1282700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>635</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>29210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>539115</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>46990</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="635" y="21791930"/>
+          <a:ext cx="8585200" cy="1511300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>414020</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>58420</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="23682960"/>
+          <a:ext cx="14312900" cy="6032500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -908,7 +1076,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8362950" cy="7543800"/>
+          <a:ext cx="8911590" cy="9387840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1176,11 +1344,11 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="S76" sqref="S76"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1198,7 +1366,7 @@
       <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1216,7 +1384,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
June 17, 2024, 06:26 PM
</commit_message>
<xml_diff>
--- a/NOTE.xlsx
+++ b/NOTE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11500"/>
+    <workbookView windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,16 +31,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -48,7 +48,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -56,14 +56,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -71,7 +71,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -79,7 +79,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -87,7 +87,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -95,7 +95,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -103,14 +103,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -118,7 +118,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -126,7 +126,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -134,14 +134,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -149,42 +149,42 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -494,19 +494,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -645,55 +645,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -734,8 +734,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="447675" y="1655445"/>
-          <a:ext cx="6174105" cy="2095500"/>
+          <a:off x="447675" y="1362075"/>
+          <a:ext cx="5762625" cy="1676400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -776,8 +776,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="628650" y="3973830"/>
-          <a:ext cx="5461635" cy="1251585"/>
+          <a:off x="628650" y="3219450"/>
+          <a:ext cx="5095875" cy="1000125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -818,8 +818,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="731520" y="5974080"/>
-          <a:ext cx="3345180" cy="1986915"/>
+          <a:off x="685800" y="4800600"/>
+          <a:ext cx="3162300" cy="1609725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -860,8 +860,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="635" y="10390505"/>
-          <a:ext cx="11372850" cy="5680710"/>
+          <a:off x="635" y="8378825"/>
+          <a:ext cx="10687050" cy="4549140"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -902,8 +902,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="15575280"/>
-          <a:ext cx="7607300" cy="5803900"/>
+          <a:off x="0" y="12515850"/>
+          <a:ext cx="7150100" cy="4672330"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -944,8 +944,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="420370" y="8434705"/>
-          <a:ext cx="14541500" cy="1282700"/>
+          <a:off x="420370" y="6800215"/>
+          <a:ext cx="13627100" cy="1031240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -986,8 +986,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="635" y="21791930"/>
-          <a:ext cx="8585200" cy="1511300"/>
+          <a:off x="635" y="17517110"/>
+          <a:ext cx="8082280" cy="1217930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1028,8 +1028,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="23682960"/>
-          <a:ext cx="14312900" cy="6032500"/>
+          <a:off x="0" y="19030950"/>
+          <a:ext cx="13444220" cy="4859020"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1076,7 +1076,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8911590" cy="9387840"/>
+          <a:ext cx="8362950" cy="7543800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1344,11 +1344,11 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="S143" sqref="S143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1366,7 +1366,7 @@
       <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1384,7 +1384,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
June 20, 2024, 06:30 PM
</commit_message>
<xml_diff>
--- a/NOTE.xlsx
+++ b/NOTE.xlsx
@@ -1042,6 +1042,48 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="图片 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="24688800"/>
+          <a:ext cx="6381750" cy="2505075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1344,8 +1386,8 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="S143" sqref="S143"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1363,7 +1405,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="S143" sqref="S143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1381,7 +1423,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="S143" sqref="S143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
July 10, 2024, 06:19 PM
</commit_message>
<xml_diff>
--- a/NOTE.xlsx
+++ b/NOTE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255"/>
+    <workbookView windowWidth="28800" windowHeight="11805"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -708,20 +708,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPr id="11" name="图片 10"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -734,8 +734,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="447675" y="1362075"/>
-          <a:ext cx="5762625" cy="1676400"/>
+          <a:off x="685800" y="171450"/>
+          <a:ext cx="7753350" cy="4933950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -750,20 +750,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="图片 3"/>
+        <xdr:cNvPr id="12" name="图片 11"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -776,302 +776,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="628650" y="3219450"/>
-          <a:ext cx="5095875" cy="1000125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="图片 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="685800" y="4800600"/>
-          <a:ext cx="3162300" cy="1609725"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>635</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>149225</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>400685</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>69215</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="图片 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="635" y="8378825"/>
-          <a:ext cx="10687050" cy="4549140"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>43180</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="12515850"/>
-          <a:ext cx="7150100" cy="4672330"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>420370</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>113665</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>331470</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>116205</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="420370" y="6800215"/>
-          <a:ext cx="13627100" cy="1031240"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>635</xdr:colOff>
-      <xdr:row>102</xdr:row>
-      <xdr:rowOff>29210</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>539115</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>46990</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="635" y="17517110"/>
-          <a:ext cx="8082280" cy="1217930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>414020</xdr:colOff>
-      <xdr:row>139</xdr:row>
-      <xdr:rowOff>58420</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="19030950"/>
-          <a:ext cx="13444220" cy="4859020"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>144</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>158</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="图片 9"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="685800" y="24688800"/>
-          <a:ext cx="6381750" cy="2505075"/>
+          <a:off x="9267825" y="666750"/>
+          <a:ext cx="2533650" cy="1781175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1386,8 +1092,8 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>